<commit_message>
cleaning up code and adding README
</commit_message>
<xml_diff>
--- a/tables/table11.xlsx
+++ b/tables/table11.xlsx
@@ -677,69 +677,69 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Education Completed</t>
+          <t>Less than Primary</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.03</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Less than Primary</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0.31</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0.22</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0.07</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>0.02</t>
+          <t>Education Completed</t>
         </is>
       </c>
     </row>
@@ -751,47 +751,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>0.26</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0.31</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.11</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.15</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -801,14 +801,14 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.08</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>mean_secondary_completed</t>
+          <t>Secondary</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -932,131 +932,131 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Household</t>
+          <t>Household Size</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3.32</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2.87</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2.46</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>3.14</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2.73</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2.65</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2.06</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2.27</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Household Size</t>
+          <t>Lives Alone</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3.32</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.31</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.87</t>
+          <t>0.24</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.46</t>
+          <t>0.27</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>3.14</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2.73</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2.65</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2.37</t>
+          <t>0.28</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2.06</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2.27</t>
+          <t>0.31</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lives Alone</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>0.32</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0.24</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0.27</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>0.39</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>0.31</t>
+          <t>Household</t>
         </is>
       </c>
     </row>
@@ -1187,49 +1187,104 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Age Migrated</t>
+          <t>Less than 15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Less than 15</t>
+          <t>15 - 24</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.07</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1256,42 +1311,42 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>15 - 24</t>
+          <t>25 - 49</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.31</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.52</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.42</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.56</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.47</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1318,62 +1373,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>25 - 49</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>0.45</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.25</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.52</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0.42</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>0.51</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>0.47</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>Age Migrated</t>
         </is>
       </c>
     </row>
@@ -1442,49 +1442,104 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Migration Cohort</t>
+          <t>Before 1965</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.41</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Before 1965</t>
+          <t>1965 - 1979</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.41</t>
+          <t>0.28</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t>0.33</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.37</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.34</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.21</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1511,42 +1566,42 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1965 - 1979</t>
+          <t>1980 - 1999</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.33</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>0.28</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0.33</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>0.35</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>0.37</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>0.31</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1573,42 +1628,42 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1980 - 1999</t>
+          <t>After 1999</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.18</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.28</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.46</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.36</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1635,255 +1690,200 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>After 1999</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>Migration Cohort</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Acculturation</t>
+          <t>Citizen</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0.74</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Citizen</t>
+          <t>English Speakers</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.54</t>
+          <t>0.73</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.91</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.69</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.76</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0.66</t>
+          <t>0.82</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>0.87</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.74</t>
+          <t>0.93</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>English Speakers</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>79658</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.91</t>
+          <t>23021</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>8980</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>21242</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>20064</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.87</t>
+          <t>25003</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0.93</t>
+          <t>352960</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>120724</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>313063</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3165675</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>94162</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>79658</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>23021</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>8980</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>21242</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>20064</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>25003</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>352960</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>120724</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>313063</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3165675</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>94162</t>
+          <t>Acculturation</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaning up tables script
</commit_message>
<xml_diff>
--- a/tables/table11.xlsx
+++ b/tables/table11.xlsx
@@ -813,57 +813,57 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.49</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>0.47</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.39</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0.53</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0.45</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>0.65</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.59</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.6</t>
         </is>
       </c>
     </row>

</xml_diff>